<commit_message>
PSR-1442 - fix for interest in land and arms length
</commit_message>
<xml_diff>
--- a/conf/TEMPLATE - SIPP Arms length land or property.xlsx
+++ b/conf/TEMPLATE - SIPP Arms length land or property.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
   <si>
     <r>
       <rPr>
@@ -142,7 +142,7 @@
     <t>Is there a Land Registry reference in respect of the land or property?</t>
   </si>
   <si>
-    <t>If no Land Registry reference, enter reason</t>
+    <t>If 'yes' enter Land registry reference number. If 'no' enter a reason for not having a Land registry reference.</t>
   </si>
   <si>
     <t>Who was the land or property acquired from?</t>
@@ -321,16 +321,16 @@
   </si>
   <si>
     <t>Enter YES or NO.
-Mandatory question.</t>
+Mandatory question if any interest in land or property transactions have taken place within the tax year.</t>
   </si>
   <si>
     <t>Max of 160 characters.
-Mandatroy field if there is no Land Registry Reference.</t>
+Mandatory question if any interest in land or property transactions have taken place within the tax year.</t>
   </si>
   <si>
     <t>Enter name.
 Max 160 characters
-Mandatory Question.</t>
+Mandatory question if the Land Registry number is not provided.</t>
   </si>
   <si>
     <t>Enter the total amount in GBP (in pounds and pence). 
@@ -339,6 +339,10 @@
   </si>
   <si>
     <t>Enter YES or NO
+Mandatory question.</t>
+  </si>
+  <si>
+    <t>Enter YES or NO.
 Mandatory question.</t>
   </si>
   <si>
@@ -837,7 +841,7 @@
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="3" t="s">
@@ -953,13 +957,13 @@
       <c r="S2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="V2" s="9" t="s">
         <v>60</v>
       </c>
       <c r="W2" s="7" t="s">
@@ -969,49 +973,49 @@
         <v>62</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="Z2" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AA2" s="7" t="s">
         <v>47</v>
       </c>
       <c r="AB2" s="9" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AD2" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AE2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="AF2" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG2" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH2" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AI2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ2" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>65</v>
-      </c>
       <c r="AL2" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AM2" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
PSR-2045 & 2046 armsLength & outStanding Loans template update
</commit_message>
<xml_diff>
--- a/conf/TEMPLATE - SIPP Arms length land or property.xlsx
+++ b/conf/TEMPLATE - SIPP Arms length land or property.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="ioSrfQVCHqajycikeCyIA1jSCnjW1gaAc2Z0zsmQ2f0="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="wLVZmjLlGl//IAiszR09sJVKImfnVbODkHwVp6XTeec="/>
     </ext>
   </extLst>
 </workbook>
@@ -25,7 +25,7 @@
         <color theme="1"/>
         <sz val="11.0"/>
       </rPr>
-      <t xml:space="preserve">The questions in this section relate to a direct or indirect interest in arm's length land or property from a connected party. 
+      <t xml:space="preserve">The questions in this section relate to a direct or indirect interest in arm's length land or property. 
 </t>
     </r>
     <r>
@@ -586,7 +586,7 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>

</xml_diff>

<commit_message>
PSR-2045 & 2046 armsLength & outStanding Loans template update (#399)
* PSR-2045 & 2046 armsLength & outStanding Loans template update

* PSR-2045 & 2046 removed in keys
</commit_message>
<xml_diff>
--- a/conf/TEMPLATE - SIPP Arms length land or property.xlsx
+++ b/conf/TEMPLATE - SIPP Arms length land or property.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="ioSrfQVCHqajycikeCyIA1jSCnjW1gaAc2Z0zsmQ2f0="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="wLVZmjLlGl//IAiszR09sJVKImfnVbODkHwVp6XTeec="/>
     </ext>
   </extLst>
 </workbook>
@@ -25,7 +25,7 @@
         <color theme="1"/>
         <sz val="11.0"/>
       </rPr>
-      <t xml:space="preserve">The questions in this section relate to a direct or indirect interest in arm's length land or property from a connected party. 
+      <t xml:space="preserve">The questions in this section relate to a direct or indirect interest in arm's length land or property. 
 </t>
     </r>
     <r>
@@ -586,7 +586,7 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>

</xml_diff>